<commit_message>
fixed stacked bar plot to include sex, corrected truth input in stacked_plot()
</commit_message>
<xml_diff>
--- a/data/outcomes_by_age_group.xlsx
+++ b/data/outcomes_by_age_group.xlsx
@@ -10,7 +10,8 @@
     <sheet name="ESRD" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Diabetes (1=yes; 0=no)" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Hypertension (1=yes; 0=no)" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="All Combined" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="SEX" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="All Combined" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1271,7 +1272,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S10"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1287,12 +1288,12 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>No ESRD</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>ESRD</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
@@ -1302,75 +1303,15 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>ESRD_%</t>
+          <t>Female_%</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>No ESRD_%</t>
+          <t>Male_%</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Total_%</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>No Diabetes</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Diabetes</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>Total</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>Diabetes_%</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>No Diabetes_%</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>Total_%</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>No Hypertension</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>Hypertension</t>
-        </is>
-      </c>
-      <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>Total</t>
-        </is>
-      </c>
-      <c r="Q1" s="1" t="inlineStr">
-        <is>
-          <t>Hypertension_%</t>
-        </is>
-      </c>
-      <c r="R1" s="1" t="inlineStr">
-        <is>
-          <t>No Hypertension_%</t>
-        </is>
-      </c>
-      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>Total_%</t>
         </is>
@@ -1383,6 +1324,377 @@
         </is>
       </c>
       <c r="B2" t="n">
+        <v>8</v>
+      </c>
+      <c r="C2" t="n">
+        <v>8</v>
+      </c>
+      <c r="D2" t="n">
+        <v>16</v>
+      </c>
+      <c r="E2" t="n">
+        <v>50</v>
+      </c>
+      <c r="F2" t="n">
+        <v>50</v>
+      </c>
+      <c r="G2" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>30-39</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>16</v>
+      </c>
+      <c r="C3" t="n">
+        <v>12</v>
+      </c>
+      <c r="D3" t="n">
+        <v>28</v>
+      </c>
+      <c r="E3" t="n">
+        <v>56.99999999999999</v>
+      </c>
+      <c r="F3" t="n">
+        <v>43</v>
+      </c>
+      <c r="G3" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>40-49</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>27</v>
+      </c>
+      <c r="C4" t="n">
+        <v>51</v>
+      </c>
+      <c r="D4" t="n">
+        <v>78</v>
+      </c>
+      <c r="E4" t="n">
+        <v>35</v>
+      </c>
+      <c r="F4" t="n">
+        <v>65</v>
+      </c>
+      <c r="G4" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>50-59</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>38</v>
+      </c>
+      <c r="C5" t="n">
+        <v>66</v>
+      </c>
+      <c r="D5" t="n">
+        <v>104</v>
+      </c>
+      <c r="E5" t="n">
+        <v>37</v>
+      </c>
+      <c r="F5" t="n">
+        <v>63</v>
+      </c>
+      <c r="G5" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>60-69</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>63</v>
+      </c>
+      <c r="C6" t="n">
+        <v>109</v>
+      </c>
+      <c r="D6" t="n">
+        <v>172</v>
+      </c>
+      <c r="E6" t="n">
+        <v>37</v>
+      </c>
+      <c r="F6" t="n">
+        <v>63</v>
+      </c>
+      <c r="G6" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>70-79</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>73</v>
+      </c>
+      <c r="C7" t="n">
+        <v>134</v>
+      </c>
+      <c r="D7" t="n">
+        <v>207</v>
+      </c>
+      <c r="E7" t="n">
+        <v>35</v>
+      </c>
+      <c r="F7" t="n">
+        <v>65</v>
+      </c>
+      <c r="G7" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>80-89</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>53</v>
+      </c>
+      <c r="C8" t="n">
+        <v>81</v>
+      </c>
+      <c r="D8" t="n">
+        <v>134</v>
+      </c>
+      <c r="E8" t="n">
+        <v>40</v>
+      </c>
+      <c r="F8" t="n">
+        <v>60</v>
+      </c>
+      <c r="G8" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>90-99</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>3</v>
+      </c>
+      <c r="C9" t="n">
+        <v>1</v>
+      </c>
+      <c r="D9" t="n">
+        <v>4</v>
+      </c>
+      <c r="E9" t="n">
+        <v>75</v>
+      </c>
+      <c r="F9" t="n">
+        <v>25</v>
+      </c>
+      <c r="G9" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>281</v>
+      </c>
+      <c r="C10" t="n">
+        <v>462</v>
+      </c>
+      <c r="D10" t="n">
+        <v>743</v>
+      </c>
+      <c r="E10" t="n">
+        <v>38</v>
+      </c>
+      <c r="F10" t="n">
+        <v>62</v>
+      </c>
+      <c r="G10" t="n">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:Y10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>age_group</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>No ESRD</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>ESRD</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>ESRD_%</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>No ESRD_%</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Total_%</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>No Diabetes</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Diabetes</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Diabetes_%</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>No Diabetes_%</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Total_%</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>No Hypertension</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Hypertension</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Hypertension_%</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>No Hypertension_%</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>Total_%</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>Female_%</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>Male_%</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>Total_%</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>18-29</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
         <v>1</v>
       </c>
       <c r="C2" t="n">
@@ -1436,6 +1748,24 @@
       <c r="S2" t="n">
         <v>100</v>
       </c>
+      <c r="T2" t="n">
+        <v>8</v>
+      </c>
+      <c r="U2" t="n">
+        <v>8</v>
+      </c>
+      <c r="V2" t="n">
+        <v>16</v>
+      </c>
+      <c r="W2" t="n">
+        <v>50</v>
+      </c>
+      <c r="X2" t="n">
+        <v>50</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -1497,6 +1827,24 @@
       <c r="S3" t="n">
         <v>100</v>
       </c>
+      <c r="T3" t="n">
+        <v>16</v>
+      </c>
+      <c r="U3" t="n">
+        <v>12</v>
+      </c>
+      <c r="V3" t="n">
+        <v>28</v>
+      </c>
+      <c r="W3" t="n">
+        <v>56.99999999999999</v>
+      </c>
+      <c r="X3" t="n">
+        <v>43</v>
+      </c>
+      <c r="Y3" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -1558,6 +1906,24 @@
       <c r="S4" t="n">
         <v>100</v>
       </c>
+      <c r="T4" t="n">
+        <v>27</v>
+      </c>
+      <c r="U4" t="n">
+        <v>51</v>
+      </c>
+      <c r="V4" t="n">
+        <v>78</v>
+      </c>
+      <c r="W4" t="n">
+        <v>35</v>
+      </c>
+      <c r="X4" t="n">
+        <v>65</v>
+      </c>
+      <c r="Y4" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -1619,6 +1985,24 @@
       <c r="S5" t="n">
         <v>100</v>
       </c>
+      <c r="T5" t="n">
+        <v>38</v>
+      </c>
+      <c r="U5" t="n">
+        <v>66</v>
+      </c>
+      <c r="V5" t="n">
+        <v>104</v>
+      </c>
+      <c r="W5" t="n">
+        <v>37</v>
+      </c>
+      <c r="X5" t="n">
+        <v>63</v>
+      </c>
+      <c r="Y5" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -1680,6 +2064,24 @@
       <c r="S6" t="n">
         <v>100</v>
       </c>
+      <c r="T6" t="n">
+        <v>63</v>
+      </c>
+      <c r="U6" t="n">
+        <v>109</v>
+      </c>
+      <c r="V6" t="n">
+        <v>172</v>
+      </c>
+      <c r="W6" t="n">
+        <v>37</v>
+      </c>
+      <c r="X6" t="n">
+        <v>63</v>
+      </c>
+      <c r="Y6" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -1741,6 +2143,24 @@
       <c r="S7" t="n">
         <v>100</v>
       </c>
+      <c r="T7" t="n">
+        <v>73</v>
+      </c>
+      <c r="U7" t="n">
+        <v>134</v>
+      </c>
+      <c r="V7" t="n">
+        <v>207</v>
+      </c>
+      <c r="W7" t="n">
+        <v>35</v>
+      </c>
+      <c r="X7" t="n">
+        <v>65</v>
+      </c>
+      <c r="Y7" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
@@ -1802,6 +2222,24 @@
       <c r="S8" t="n">
         <v>100</v>
       </c>
+      <c r="T8" t="n">
+        <v>53</v>
+      </c>
+      <c r="U8" t="n">
+        <v>81</v>
+      </c>
+      <c r="V8" t="n">
+        <v>134</v>
+      </c>
+      <c r="W8" t="n">
+        <v>40</v>
+      </c>
+      <c r="X8" t="n">
+        <v>60</v>
+      </c>
+      <c r="Y8" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
@@ -1863,6 +2301,24 @@
       <c r="S9" t="n">
         <v>100</v>
       </c>
+      <c r="T9" t="n">
+        <v>3</v>
+      </c>
+      <c r="U9" t="n">
+        <v>1</v>
+      </c>
+      <c r="V9" t="n">
+        <v>4</v>
+      </c>
+      <c r="W9" t="n">
+        <v>75</v>
+      </c>
+      <c r="X9" t="n">
+        <v>25</v>
+      </c>
+      <c r="Y9" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
@@ -1922,6 +2378,24 @@
         <v>3</v>
       </c>
       <c r="S10" t="n">
+        <v>100</v>
+      </c>
+      <c r="T10" t="n">
+        <v>281</v>
+      </c>
+      <c r="U10" t="n">
+        <v>462</v>
+      </c>
+      <c r="V10" t="n">
+        <v>743</v>
+      </c>
+      <c r="W10" t="n">
+        <v>38</v>
+      </c>
+      <c r="X10" t="n">
+        <v>62</v>
+      </c>
+      <c r="Y10" t="n">
         <v>100</v>
       </c>
     </row>

</xml_diff>